<commit_message>
Resistance and Support stock filtering
</commit_message>
<xml_diff>
--- a/Stocks_filtered/support_resistance_scan.xlsx
+++ b/Stocks_filtered/support_resistance_scan.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,963 +459,1109 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GPPL</t>
+          <t>GRAPHITE</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>161.9329986572266</v>
+        <v>579.1500244140625</v>
       </c>
       <c r="C2" t="n">
-        <v>173.4803009033203</v>
+        <v>623.1500244140625</v>
       </c>
       <c r="D2" t="n">
-        <v>165.8800048828125</v>
+        <v>609.9000244140625</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ECLERX</t>
+          <t>GPPL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3928</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4429.2998046875</v>
-      </c>
+        <v>153.9459075927734</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>4323.89990234375</v>
+        <v>165.8800048828125</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HINDZINC</t>
+          <t>HEROMOTOCO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>655.3802490234375</v>
+        <v>5296</v>
       </c>
       <c r="C4" t="n">
-        <v>702.1829833984375</v>
+        <v>6350.5</v>
       </c>
       <c r="D4" t="n">
-        <v>698.7000122070312</v>
+        <v>5384</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GESHIP</t>
+          <t>IDFCFIRSTB</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1047.849853515625</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1133.199951171875</v>
-      </c>
+        <v>81.76999664306641</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1108.800048828125</v>
+        <v>82.98999786376953</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>360ONE</t>
+          <t>INDIACEM</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1080.639770507812</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1239.097900390625</v>
-      </c>
+        <v>398.7000122070312</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1112.300048828125</v>
+        <v>431.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INDIACEM</t>
+          <t>INDIANB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>398.7000122070312</v>
+        <v>873.9500122070312</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>431.5</v>
+        <v>876.4500122070312</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LAURUSLABS</t>
+          <t>IKS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>931.3314819335938</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
+        <v>1487.199951171875</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1745.5</v>
+      </c>
       <c r="D8" t="n">
-        <v>1016.400024414062</v>
+        <v>1651.099975585938</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SAIL</t>
+          <t>JSWSTEEL</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>141.9900054931641</v>
+        <v>1060.344604492188</v>
       </c>
       <c r="C9" t="n">
-        <v>166.1107177734375</v>
+        <v>1206</v>
       </c>
       <c r="D9" t="n">
-        <v>149.0299987792969</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>APOLLOTYRE</t>
+          <t>JAMNAAUTO</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>490.5232543945312</v>
-      </c>
-      <c r="C10" t="n">
-        <v>521.4500122070312</v>
-      </c>
+        <v>106.8753356933594</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>499.2000122070312</v>
+        <v>116.4300003051758</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NLCINDIA</t>
+          <t>JINDALSTEL</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>242.5510711669922</v>
+        <v>1002.884918212891</v>
       </c>
       <c r="C11" t="n">
-        <v>253.7799936930338</v>
+        <v>1076.349975585938</v>
       </c>
       <c r="D11" t="n">
-        <v>247.1000061035156</v>
+        <v>1063.599975585938</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CHENNPETRO</t>
+          <t>KARURVYSYA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>831.6135864257812</v>
-      </c>
-      <c r="C12" t="n">
-        <v>874.8945922851562</v>
-      </c>
+        <v>245.3600006103516</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>842.2000122070312</v>
+        <v>265.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HEG</t>
+          <t>CHENNPETRO</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>521.4956970214844</v>
+        <v>773.69140625</v>
       </c>
       <c r="C13" t="n">
-        <v>537.3853149414062</v>
+        <v>1029</v>
       </c>
       <c r="D13" t="n">
-        <v>528.9000244140625</v>
+        <v>842.2000122070312</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IDEA</t>
+          <t>CRAFTSMAN</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9.575000286102295</v>
-      </c>
-      <c r="C14" t="n">
-        <v>10.89999961853027</v>
-      </c>
+        <v>7093</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>9.930000305175781</v>
+        <v>7198.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BSE</t>
+          <t>DYNAMATECH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2482</v>
+        <v>7266</v>
       </c>
       <c r="C15" t="n">
-        <v>2902.39990234375</v>
+        <v>9715</v>
       </c>
       <c r="D15" t="n">
-        <v>2685.39990234375</v>
+        <v>7899.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BHARATFORG</t>
+          <t>EMCURE</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1314.5</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1568.472900390625</v>
-      </c>
+        <v>1493.099975585938</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>1408.800048828125</v>
+        <v>1530.800048828125</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>JBCHEPHARM</t>
+          <t>FIEMIND</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1831.575439453125</v>
+        <v>1933.699951171875</v>
       </c>
       <c r="C17" t="n">
-        <v>1870.979919433594</v>
+        <v>2148.10009765625</v>
       </c>
       <c r="D17" t="n">
-        <v>1846</v>
+        <v>2145.60009765625</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MANAPPURAM</t>
+          <t>GPIL</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>290.6686401367188</v>
-      </c>
-      <c r="C18" t="inlineStr"/>
+        <v>232.9400024414062</v>
+      </c>
+      <c r="C18" t="n">
+        <v>283.739990234375</v>
+      </c>
       <c r="D18" t="n">
-        <v>294.75</v>
+        <v>241.8500061035156</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3MINDIA</t>
+          <t>GRANULES</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>31706.59765625</v>
+        <v>544.2000122070312</v>
       </c>
       <c r="C19" t="n">
-        <v>35836.48046875</v>
+        <v>569.5499877929688</v>
       </c>
       <c r="D19" t="n">
-        <v>33315</v>
+        <v>565</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GMDCLTD</t>
+          <t>GESHIP</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>488.8999938964844</v>
+        <v>1047.849853515625</v>
       </c>
       <c r="C20" t="n">
-        <v>613.0999755859375</v>
+        <v>1133.199951171875</v>
       </c>
       <c r="D20" t="n">
-        <v>518.7999877929688</v>
+        <v>1108.800048828125</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>UJJIVANSFB</t>
+          <t>GMDCLTD</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>57.96752548217773</v>
-      </c>
-      <c r="C21" t="inlineStr"/>
+        <v>488.8999938964844</v>
+      </c>
+      <c r="C21" t="n">
+        <v>613.0999755859375</v>
+      </c>
       <c r="D21" t="n">
-        <v>63.06000137329102</v>
+        <v>518.7999877929688</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MRPL</t>
+          <t>IOC</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>150.8699951171875</v>
+        <v>143.9965515136719</v>
       </c>
       <c r="C22" t="n">
-        <v>172.4900054931641</v>
+        <v>166.1581268310547</v>
       </c>
       <c r="D22" t="n">
-        <v>155.3999938964844</v>
+        <v>156.0299987792969</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RBLBANK</t>
+          <t>INFY</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>265.8829345703125</v>
-      </c>
-      <c r="C23" t="n">
-        <v>289.4916687011719</v>
-      </c>
+        <v>1615.96142578125</v>
+      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>288.6000061035156</v>
+        <v>1670.800048828125</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>M&amp;MFIN</t>
+          <t>JBCHEPHARM</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>325.4159240722656</v>
+        <v>1794.404663085938</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>360.6499938964844</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>IDBI</t>
+          <t>CCL</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>97.40000152587891</v>
+        <v>918</v>
       </c>
       <c r="C25" t="n">
-        <v>99.19779968261719</v>
+        <v>1053.099975585938</v>
       </c>
       <c r="D25" t="n">
-        <v>97.41999816894531</v>
+        <v>925.6500244140625</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MAHABANK</t>
+          <t>CANFINHOME</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>64.72964477539062</v>
-      </c>
-      <c r="C26" t="n">
-        <v>65.99117279052734</v>
-      </c>
+        <v>810.806884765625</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
-        <v>65.62999725341797</v>
+        <v>898.0999755859375</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GPIL</t>
+          <t>FORCEMOT</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>235.3400268554688</v>
+        <v>18194</v>
       </c>
       <c r="C27" t="n">
-        <v>257.7935791015625</v>
+        <v>20169.470703125</v>
       </c>
       <c r="D27" t="n">
-        <v>241.8500061035156</v>
+        <v>19325</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GRANULES</t>
+          <t>360ONE</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>544.2000122070312</v>
+        <v>1065.400024414062</v>
       </c>
       <c r="C28" t="n">
-        <v>569.5499877929688</v>
+        <v>1239.097900390625</v>
       </c>
       <c r="D28" t="n">
-        <v>565</v>
+        <v>1112.300048828125</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>IIFL</t>
+          <t>ANANDRATHI</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>499.7615356445312</v>
+        <v>2855.89990234375</v>
       </c>
       <c r="C29" t="n">
-        <v>523.0999755859375</v>
+        <v>3125.10009765625</v>
       </c>
       <c r="D29" t="n">
-        <v>521.1500244140625</v>
+        <v>2959.39990234375</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PERSISTENT</t>
+          <t>ANURAS</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>6090.08056640625</v>
-      </c>
-      <c r="C30" t="n">
-        <v>6438.8994140625</v>
-      </c>
+        <v>1158.400024414062</v>
+      </c>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>6155</v>
+        <v>1230.199951171875</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CANFINHOME</t>
+          <t>APOLLOTYRE</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>890.9421997070312</v>
+        <v>489.4623107910156</v>
       </c>
       <c r="C31" t="n">
-        <v>910.6213989257812</v>
+        <v>521.4500122070312</v>
       </c>
       <c r="D31" t="n">
-        <v>898.0999755859375</v>
+        <v>499.2000122070312</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GRAPHITE</t>
+          <t>BAJAJ-AUTO</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>578.4350280761719</v>
-      </c>
-      <c r="C32" t="n">
-        <v>623.1500244140625</v>
-      </c>
+        <v>9117.5</v>
+      </c>
+      <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>609.9000244140625</v>
+        <v>9413.5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>IDFCFIRSTB</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>82.49918619791667</v>
+        <v>389.4500122070312</v>
       </c>
       <c r="C33" t="n">
-        <v>84.52335357666016</v>
+        <v>426.7052154541016</v>
       </c>
       <c r="D33" t="n">
-        <v>82.98999786376953</v>
+        <v>410.7000122070312</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ANANDRATHI</t>
+          <t>BPCL</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2855.89990234375</v>
+        <v>334.1123046875</v>
       </c>
       <c r="C34" t="n">
-        <v>3125.10009765625</v>
+        <v>371.1499938964844</v>
       </c>
       <c r="D34" t="n">
-        <v>2959.39990234375</v>
+        <v>349.1499938964844</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>KIRLOSENG</t>
+          <t>EICHERMOT</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1007.467102050781</v>
+        <v>6695</v>
       </c>
       <c r="C35" t="n">
-        <v>1168.528930664062</v>
+        <v>7047</v>
       </c>
       <c r="D35" t="n">
-        <v>1094.199951171875</v>
+        <v>6973</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CRAFTSMAN</t>
+          <t>HEG</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>7093</v>
-      </c>
-      <c r="C36" t="inlineStr"/>
+        <v>521.4956970214844</v>
+      </c>
+      <c r="C36" t="n">
+        <v>537.3853149414062</v>
+      </c>
       <c r="D36" t="n">
-        <v>7198.5</v>
+        <v>528.9000244140625</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>INDIANB</t>
+          <t>IDBI</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>873.9500122070312</v>
-      </c>
-      <c r="C37" t="inlineStr"/>
+        <v>97.40000152587891</v>
+      </c>
+      <c r="C37" t="n">
+        <v>99.19779968261719</v>
+      </c>
       <c r="D37" t="n">
-        <v>876.4500122070312</v>
+        <v>97.41999816894531</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CCL</t>
+          <t>IIFLCAPS</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>918</v>
+        <v>322.4500122070312</v>
       </c>
       <c r="C38" t="n">
-        <v>1053.099975585938</v>
+        <v>347.8999938964844</v>
       </c>
       <c r="D38" t="n">
-        <v>925.6500244140625</v>
+        <v>333</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BPCL</t>
+          <t>3MINDIA</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>347.6072387695312</v>
+        <v>31615</v>
       </c>
       <c r="C39" t="n">
-        <v>371.1499938964844</v>
+        <v>35910</v>
       </c>
       <c r="D39" t="n">
-        <v>349.1499938964844</v>
+        <v>33315</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CHOLAFIN</t>
+          <t>AETHER</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1606.76318359375</v>
-      </c>
-      <c r="C40" t="n">
-        <v>1653.35595703125</v>
-      </c>
+        <v>916.0249938964844</v>
+      </c>
+      <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
-        <v>1643.199951171875</v>
+        <v>968.3499755859375</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TORNTPHARM</t>
+          <t>ASAHIINDIA</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3831.800048828125</v>
-      </c>
-      <c r="C41" t="inlineStr"/>
+        <v>849.680908203125</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1027.099975585938</v>
+      </c>
       <c r="D41" t="n">
-        <v>3932.199951171875</v>
+        <v>942.9000244140625</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TVSMOTOR</t>
+          <t>BSE</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>3386.5</v>
+        <v>2482</v>
       </c>
       <c r="C42" t="n">
-        <v>3654</v>
+        <v>2902.39990234375</v>
       </c>
       <c r="D42" t="n">
-        <v>3549.800048828125</v>
+        <v>2685.39990234375</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>^CNXMETAL</t>
+          <t>BHARATFORG</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>10612.150390625</v>
+        <v>1314.5</v>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="n">
-        <v>11477.7998046875</v>
+        <v>1408.800048828125</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>^CNXAUTO</t>
+          <t>LAURUSLABS</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>26250.69921875</v>
-      </c>
-      <c r="C44" t="n">
-        <v>27610.75</v>
-      </c>
+        <v>931.3314819335938</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>26804.55078125</v>
+        <v>1016.400024414062</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>NMDC</t>
+          <t>LUMAXTECH</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>75.50038909912109</v>
-      </c>
-      <c r="C45" t="n">
-        <v>77.12999725341797</v>
-      </c>
+        <v>1302.599975585938</v>
+      </c>
+      <c r="C45" t="inlineStr"/>
       <c r="D45" t="n">
-        <v>76.36000061035156</v>
+        <v>1377.599975585938</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>KARURVYSYA</t>
+          <t>NLCINDIA</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>245.3600006103516</v>
-      </c>
-      <c r="C46" t="inlineStr"/>
+        <v>236.9298858642578</v>
+      </c>
+      <c r="C46" t="n">
+        <v>252.3873596191406</v>
+      </c>
       <c r="D46" t="n">
-        <v>265.5</v>
+        <v>247.1000061035156</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ASAHIINDIA</t>
+          <t>NMDC</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>849.680908203125</v>
+        <v>73.51000213623047</v>
       </c>
       <c r="C47" t="n">
-        <v>1027.099975585938</v>
+        <v>77.12999725341797</v>
       </c>
       <c r="D47" t="n">
-        <v>942.9000244140625</v>
+        <v>76.36000061035156</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PNB</t>
+          <t>PTCIL</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>119.0051956176758</v>
+        <v>17083.150390625</v>
       </c>
       <c r="C48" t="n">
-        <v>125.0082702636719</v>
+        <v>18875</v>
       </c>
       <c r="D48" t="n">
-        <v>120.1500015258789</v>
+        <v>17478</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>TATASTEEL</t>
+          <t>PRICOLLTD</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>182.8399963378906</v>
+        <v>538.1710205078125</v>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
-        <v>187.6100006103516</v>
+        <v>581.5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>TITAN</t>
+          <t>PRIVISCL</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3790.018310546875</v>
-      </c>
-      <c r="C50" t="inlineStr"/>
+        <v>2479.699951171875</v>
+      </c>
+      <c r="C50" t="n">
+        <v>3388</v>
+      </c>
       <c r="D50" t="n">
-        <v>4021.800048828125</v>
+        <v>2717.39990234375</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>EICHERMOT</t>
+          <t>PNB</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>6695</v>
-      </c>
-      <c r="C51" t="n">
-        <v>7047</v>
-      </c>
+        <v>117.8099975585938</v>
+      </c>
+      <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
-        <v>6973</v>
+        <v>120.1500015258789</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>MOTHERSON</t>
+          <t>RBLBANK</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>104.2743377685547</v>
+        <v>263.2029113769531</v>
       </c>
       <c r="C52" t="n">
-        <v>109.0800018310547</v>
+        <v>328.25</v>
       </c>
       <c r="D52" t="n">
-        <v>108.4000015258789</v>
+        <v>288.6000061035156</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>IOC</t>
+          <t>SBILIFE</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>146.7690887451172</v>
-      </c>
-      <c r="C53" t="n">
-        <v>156.3865814208984</v>
-      </c>
+        <v>1854.799987792969</v>
+      </c>
+      <c r="C53" t="inlineStr"/>
       <c r="D53" t="n">
-        <v>156.0299987792969</v>
+        <v>2002.599975585938</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>BANKBARODA</t>
+          <t>SAGILITY</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>269.1988525390625</v>
-      </c>
-      <c r="C54" t="inlineStr"/>
+        <v>46.73328399658203</v>
+      </c>
+      <c r="C54" t="n">
+        <v>53.27999877929688</v>
+      </c>
       <c r="D54" t="n">
-        <v>296.1499938964844</v>
+        <v>51.68999862670898</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>LTIM</t>
+          <t>MOTHERSON</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>5631.55029296875</v>
+        <v>104.2743377685547</v>
       </c>
       <c r="C55" t="n">
-        <v>6138.54736328125</v>
+        <v>109.0800018310547</v>
       </c>
       <c r="D55" t="n">
-        <v>5893.5</v>
+        <v>108.4000015258789</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>INFY</t>
+          <t>SHRIPISTON</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>1609.019592285156</v>
+        <v>2595.89990234375</v>
       </c>
       <c r="C56" t="n">
-        <v>1709.532165527344</v>
+        <v>2733.199951171875</v>
       </c>
       <c r="D56" t="n">
-        <v>1670.800048828125</v>
+        <v>2700.300048828125</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>HEROMOTOCO</t>
+          <t>TATASTEEL</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>5296</v>
-      </c>
-      <c r="C57" t="n">
-        <v>5537.1416015625</v>
-      </c>
+        <v>182.8399963378906</v>
+      </c>
+      <c r="C57" t="inlineStr"/>
       <c r="D57" t="n">
-        <v>5384</v>
+        <v>187.6100006103516</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BAJAJ-AUTO</t>
+          <t>SANDUMA</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>9129.683268229166</v>
+        <v>201.9700012207031</v>
       </c>
       <c r="C58" t="n">
-        <v>9715.5205078125</v>
+        <v>222.5</v>
       </c>
       <c r="D58" t="n">
-        <v>9413.5</v>
+        <v>205.3300018310547</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>SANSERA</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>389.4500122070312</v>
-      </c>
-      <c r="C59" t="n">
-        <v>426.7052154541016</v>
-      </c>
+        <v>1495</v>
+      </c>
+      <c r="C59" t="inlineStr"/>
       <c r="D59" t="n">
-        <v>410.7000122070312</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SBILIFE</t>
+          <t>SEQUENT</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1892.69775390625</v>
-      </c>
-      <c r="C60" t="inlineStr"/>
+        <v>197.2599945068359</v>
+      </c>
+      <c r="C60" t="n">
+        <v>238.7299957275391</v>
+      </c>
       <c r="D60" t="n">
-        <v>2002.599975585938</v>
+        <v>207.1600036621094</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>JINDALSTEL</t>
+          <t>TORNTPHARM</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1029.058471679688</v>
-      </c>
-      <c r="C61" t="n">
-        <v>1075.190551757812</v>
-      </c>
+        <v>3831.800048828125</v>
+      </c>
+      <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
-        <v>1063.599975585938</v>
+        <v>3932.199951171875</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>JSWSTEEL</t>
+          <t>TITAN</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1060.344604492188</v>
-      </c>
-      <c r="C62" t="n">
-        <v>1206</v>
-      </c>
+        <v>3670.56884765625</v>
+      </c>
+      <c r="C62" t="inlineStr"/>
       <c r="D62" t="n">
-        <v>1170</v>
+        <v>4021.800048828125</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>LTIM</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>5407.736328125</v>
+      </c>
+      <c r="C63" t="n">
+        <v>6292</v>
+      </c>
+      <c r="D63" t="n">
+        <v>5893.5</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>MRPL</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>150.8699951171875</v>
+      </c>
+      <c r="C64" t="n">
+        <v>172.4900054931641</v>
+      </c>
+      <c r="D64" t="n">
+        <v>155.3999938964844</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>MANAPPURAM</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>290.6686401367188</v>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>294.75</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>PERSISTENT</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>6090.08056640625</v>
+      </c>
+      <c r="C66" t="n">
+        <v>6520.5</v>
+      </c>
+      <c r="D66" t="n">
+        <v>6155</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>SAIL</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>141.9900054931641</v>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>149.0299987792969</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>TVSMOTOR</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>3386.5</v>
+      </c>
+      <c r="C68" t="n">
+        <v>3654</v>
+      </c>
+      <c r="D68" t="n">
+        <v>3549.800048828125</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>THANGAMAYL</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>3389.300048828125</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>THYROCARE</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>410.0499877929688</v>
+      </c>
+      <c r="C70" t="n">
+        <v>458.6543579101562</v>
+      </c>
+      <c r="D70" t="n">
+        <v>440.25</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ECLERX</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>3928</v>
+      </c>
+      <c r="C71" t="n">
+        <v>4429.2998046875</v>
+      </c>
+      <c r="D71" t="n">
+        <v>4323.89990234375</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>^CNXMETAL</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>10612.150390625</v>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>11477.7998046875</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
           <t>^CNXPSUBANK</t>
         </is>
       </c>
-      <c r="B63" t="n">
+      <c r="B73" t="n">
         <v>8247.7998046875</v>
       </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="n">
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="n">
         <v>8781.0498046875</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>IDEA</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>9.600000381469727</v>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="n">
+        <v>9.930000305175781</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1462,317 +1608,537 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MUTHOOTFIN</t>
+          <t>HINDALCO</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2662.800048828125</v>
+        <v>847.8499755859375</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>3802.800048828125</v>
+        <v>950.2999877929688</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LTF</t>
+          <t>JKTYRE</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>205.6300048828125</v>
+        <v>379.6864624023438</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>288</v>
+        <v>508.0499877929688</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FEDERALBNK</t>
+          <t>LTF</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>213.0701675415039</v>
+        <v>205.6300048828125</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>278.5499877929688</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AUBANK</t>
+          <t>CEATLTD</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>821</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
+        <v>3091.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3793.610107421875</v>
+      </c>
       <c r="D5" t="n">
-        <v>966.0999755859375</v>
+        <v>3718.199951171875</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ASHOKLEY</t>
+          <t>CHOLAFIN</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>140.9739074707031</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+        <v>1420.699951171875</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1653.35595703125</v>
+      </c>
       <c r="D6" t="n">
-        <v>192.9799957275391</v>
+        <v>1643.199951171875</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ABCAPITAL</t>
+          <t>CUB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>275.0499877929688</v>
-      </c>
-      <c r="C7" t="n">
-        <v>362.9500122070312</v>
-      </c>
+        <v>215.2420959472656</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>347.4500122070312</v>
+        <v>275.4500122070312</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NATIONALUM</t>
+          <t>DCBBANK</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>240.9099731445312</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
+        <v>146.3274612426758</v>
+      </c>
+      <c r="C8" t="n">
+        <v>186.0700073242188</v>
+      </c>
       <c r="D8" t="n">
-        <v>370.6499938964844</v>
+        <v>182.8999938964844</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MCX</t>
+          <t>KIRLOSENG</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1770.139526367188</v>
+        <v>964.6500244140625</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>2282</v>
+        <v>1094.199951171875</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CUB</t>
+          <t>CSBBANK</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>215.2420959472656</v>
+        <v>431.75</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>275.4500122070312</v>
+        <v>488.3999938964844</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HINDCOPPER</t>
+          <t>CANBK</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>387.8765258789062</v>
+        <v>114.4499969482422</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>535.9000244140625</v>
+        <v>151.8099975585938</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NAVINFLUOR</t>
+          <t>FEDERALBNK</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5046.4501953125</v>
+        <v>214.0243988037109</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>5919</v>
+        <v>278.5499877929688</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BANKINDIA</t>
+          <t>IIFL</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>142.422004699707</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
+        <v>427.2000122070312</v>
+      </c>
+      <c r="C13" t="n">
+        <v>532.9500122070312</v>
+      </c>
       <c r="D13" t="n">
-        <v>159.6499938964844</v>
+        <v>521.1500244140625</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>ABCAPITAL</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>13351.095703125</v>
+        <v>275.0499877929688</v>
       </c>
       <c r="C14" t="n">
-        <v>15479</v>
+        <v>362.9500122070312</v>
       </c>
       <c r="D14" t="n">
-        <v>15469</v>
+        <v>347.4500122070312</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>JKTYRE</t>
+          <t>ASHOKLEY</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>449.17236328125</v>
-      </c>
-      <c r="C15" t="n">
-        <v>514.7578735351562</v>
-      </c>
+        <v>140.9739074707031</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>508.0499877929688</v>
+        <v>192.9799957275391</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CEATLTD</t>
+          <t>HINDZINC</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3221.4580078125</v>
-      </c>
-      <c r="C16" t="n">
-        <v>3793.610107421875</v>
-      </c>
+        <v>502.2373352050781</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>3718.199951171875</v>
+        <v>698.7000122070312</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CANBK</t>
+          <t>HINDCOPPER</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>117.1212158203125</v>
+        <v>344.5499877929688</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>151.8099975585938</v>
+        <v>535.9000244140625</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>UNIONBANK</t>
+          <t>AUBANK</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>150.9372711181641</v>
+        <v>821</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>172.7700042724609</v>
+        <v>966.0999755859375</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SBIN</t>
+          <t>BANKBARODA</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>871.84375</v>
+        <v>245.4449996948242</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>1029.5</v>
+        <v>296.1499938964844</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>VEDL</t>
+          <t>MAHABANK</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>484.3845520019531</v>
+        <v>58.72708129882812</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>684.1500244140625</v>
+        <v>65.62999725341797</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SHRIRAMFIN</t>
+          <t>BANKINDIA</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>708.3565063476562</v>
+        <v>120.0254058837891</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1003.549987792969</v>
+        <v>159.6499938964844</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>M&amp;M</t>
+          <t>MTARTECH</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3165.6171875</v>
-      </c>
-      <c r="C22" t="inlineStr"/>
+        <v>1770.699951171875</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2626.60009765625</v>
+      </c>
       <c r="D22" t="n">
-        <v>3543.39990234375</v>
+        <v>2400.199951171875</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>HINDALCO</t>
+          <t>M&amp;M</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>847.8499755859375</v>
+        <v>3172.958251953125</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>950.2999877929688</v>
+        <v>3543.39990234375</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>MUTHOOTFIN</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2662.800048828125</v>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>3802.800048828125</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>NAVINFLUOR</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>5046.4501953125</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>5919</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>NATIONALUM</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>188.5459747314453</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>370.6499938964844</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>RRKABEL</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1164.160400390625</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1412.923828125</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1351.599975585938</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SOUTHBANK</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>30.26901626586914</v>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>UJJIVANSFB</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>49.06999969482422</v>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>63.06000137329102</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>UNIONBANK</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>148.2577209472656</v>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>172.7700042724609</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>M&amp;MFIN</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>290.4837341308594</v>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>360.6499938964844</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>MARUTI</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>12882.814453125</v>
+      </c>
+      <c r="C32" t="n">
+        <v>15479</v>
+      </c>
+      <c r="D32" t="n">
+        <v>15469</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>MCX</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1770.139526367188</v>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>RATEGAIN</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>505.0499877929688</v>
+      </c>
+      <c r="C34" t="n">
+        <v>638.25</v>
+      </c>
+      <c r="D34" t="n">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>SHRIRAMFIN</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>692.6035766601562</v>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>1003.549987792969</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>SBIN</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>813.0499877929688</v>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>1029.5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>^CNXAUTO</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>23980.5498046875</v>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>26804.55078125</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>VEDL</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>445.4774475097656</v>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>684.1500244140625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>